<commit_message>
fixed issue with dac struct
</commit_message>
<xml_diff>
--- a/deps/hdacv2_characterization/analog_amplitude_vs_frequency_v2.xlsx
+++ b/deps/hdacv2_characterization/analog_amplitude_vs_frequency_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18280" yWindow="60" windowWidth="28800" windowHeight="17460" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Global crossbar" sheetId="1" r:id="rId1"/>
@@ -106,10 +106,10 @@
     <t>multiplier 1x (us)</t>
   </si>
   <si>
-    <t>fanout (1x/10x) [degrees]</t>
+    <t>other [degrees]</t>
   </si>
   <si>
-    <t>fanout (1x/10x) time</t>
+    <t>other time</t>
   </si>
 </sst>
 </file>
@@ -5698,8 +5698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7044,7 +7044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -7214,7 +7214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>

</xml_diff>